<commit_message>
Uporządkowano repozytorium i dodano displayCreator.js
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.sarapata\Desktop\CreativeCreator - LinkTXT - automatyczny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.sarapata\Desktop\CreativeCreator - Display\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{286699D2-71D3-492F-8A66-E21A992BA6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741125D3-25E7-4EBE-A4FE-1A4B1D0B79B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51465" yWindow="-16230" windowWidth="25095" windowHeight="20505" xr2:uid="{268508D8-A5A5-43C6-B277-EABFD88C5871}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>advertiserId</t>
   </si>
@@ -39,7 +39,7 @@
     <t>targetUrl</t>
   </si>
   <si>
-    <t>Łap co chcesz z tańszą dostawą na TaniaKsiazka.pl. Dostawa za 6,99 zł. Tylko do 29 lipca</t>
+    <t>displays</t>
   </si>
   <si>
     <t>do 29.07</t>
@@ -48,19 +48,28 @@
     <t>https://www.taniaksiazka.pl/t/dostawa</t>
   </si>
   <si>
-    <t>Zabierz kryminał na urlop. Druga książka 55% taniej od ceny okładkowej, tylko teraz na TaniaKsiazka.pl!</t>
+    <t>Misja? Wakacje bez nudy! Sprawdź letnie okazje cenowe na książki, gry i zabawki na TaniaKsiazka.pl</t>
   </si>
   <si>
     <t>do 31.07</t>
   </si>
   <si>
-    <t>https://www.taniaksiazka.pl/akcja/id-5118</t>
-  </si>
-  <si>
-    <t>Kup wyprawkę szkolną teraz z tańszą dostawą</t>
-  </si>
-  <si>
-    <t>https://www.taniaksiazka.pl/wyprawka-szkolna-a-672.html</t>
+    <t>https://www.taniaksiazka.pl/letnia-kraina-zabaw-a-1185.html</t>
+  </si>
+  <si>
+    <t>Ceny topnieją okazje szaleją. Złap książki już od 5,99 zł na TaniaKsiazka.pl</t>
+  </si>
+  <si>
+    <t>https://www.taniaksiazka.pl/images/afiliacjaTK/banery/2025/LetniaWyprzedaz2025.zip</t>
+  </si>
+  <si>
+    <t>Książka na fali - czytaj na wakacje z TaniaKsiazka.pl. Skompletuj swój wakacyjny pakiet: 2 ksiażki za 50 zł lub 2 ksiażki za 60 zł</t>
+  </si>
+  <si>
+    <t>https://www.taniaksiazka.pl/t/ksiazka-na-wakacje</t>
+  </si>
+  <si>
+    <t>https://www.taniaksiazka.pl/images/afiliacjaTK/banery/2025/KsiazkaNaFali.zip</t>
   </si>
 </sst>
 </file>
@@ -93,18 +102,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEDF1F3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,11 +123,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -442,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F9F985-434F-4E05-A84D-217602AF6B5D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,7 +455,7 @@
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,54 +468,60 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="57" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>88278</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>88278</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
+      <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>88278</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{ABEB3644-484C-4E41-83E2-CE29CFB10000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{D2E2C760-8A80-4936-BA22-EB22FECD566A}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{F47A080D-93F2-480D-B82B-2461348AE819}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6AEE9E32-0AFC-48EB-96D5-A940EC408446}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{775237C0-07FB-466A-B358-02B646F0ED2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>